<commit_message>
Rename variables, change URI format
</commit_message>
<xml_diff>
--- a/evaluation/v2/evalute.xlsx
+++ b/evaluation/v2/evalute.xlsx
@@ -1399,343 +1399,343 @@
     <t>Gl 02</t>
   </si>
   <si>
-    <t>WardahEverydayCheekLiptint</t>
-  </si>
-  <si>
-    <t>WardahExclusiveMatteLipCream</t>
-  </si>
-  <si>
-    <t>WardahEyexpertEyeLipMakeUpRemover</t>
-  </si>
-  <si>
-    <t>WardahIntenseMatteLipstick</t>
-  </si>
-  <si>
-    <t>WardahLipstickLonglasting</t>
-  </si>
-  <si>
-    <t>WardahLonglastingLipstick</t>
-  </si>
-  <si>
-    <t>WardahEyexpertOptimumHiBlackLiner</t>
-  </si>
-  <si>
-    <t>WardahEyexpertAquaLashMascara</t>
-  </si>
-  <si>
-    <t>WardahEyexpertEyeShadowClassic</t>
-  </si>
-  <si>
-    <t>WardahEyexpertTheVolumeExpertMascara</t>
-  </si>
-  <si>
-    <t>WardahRenewYouAntiAgingEyeCream</t>
-  </si>
-  <si>
-    <t>WardahEyexpertPerfectcurlMascara</t>
-  </si>
-  <si>
-    <t>WardahEyexpertStaylastLiquidEyeliner</t>
-  </si>
-  <si>
-    <t>WardahEyeShadow</t>
-  </si>
-  <si>
-    <t>WardahEyexpertEyeShadow</t>
-  </si>
-  <si>
-    <t>WardahAcnedermFacePowder</t>
-  </si>
-  <si>
-    <t>WardahBlushOn</t>
-  </si>
-  <si>
-    <t>WardahExclusiveLiquidFoundation</t>
-  </si>
-  <si>
-    <t>WardahExclusiveTwoWayCake</t>
-  </si>
-  <si>
-    <t>WardahEverydayLuminousCompactPowder</t>
-  </si>
-  <si>
-    <t>WardahEverydayLuminousFacePowder</t>
-  </si>
-  <si>
-    <t>WardahRefillLighteningPowderFoundationLightFeel</t>
-  </si>
-  <si>
-    <t>WardahLighteningPowderFoundationLightFeel</t>
-  </si>
-  <si>
-    <t>WardahRefillExclusiveTwoWayCake</t>
-  </si>
-  <si>
-    <t>WardahLighteningPowderFoundation</t>
-  </si>
-  <si>
-    <t>WardahRefillLighteningPowderFoundation</t>
-  </si>
-  <si>
-    <t>WardahEverydayLuminousLiquidFoundation</t>
-  </si>
-  <si>
-    <t>WardahRefillEverydayLuminousTwoWayCake</t>
-  </si>
-  <si>
-    <t>WardahEverydayShineFreeBbLoosePowder</t>
-  </si>
-  <si>
-    <t>WardahLighteningMattePowder</t>
-  </si>
-  <si>
-    <t>WardahLighteningBbCakePowder</t>
-  </si>
-  <si>
-    <t>WardahEverydayLuminousTwoWayCake</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectPorefectionSkinPrimer</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectMineralightMatteBbCushion</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectSpotlightChromaticEyePalette</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectGeniustwistMaticContourBrowBrushed</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectHypergeticPreciseBlackLiner</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectMattesetterLipMattePaint</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectQuickFixCoverCorrectConcealer</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectDynamaticMicrosmoothLiner</t>
-  </si>
-  <si>
-    <t>WardahRefillInstaperfectMineralightMatteBbCushion</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectGlossChicLipCrayon</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectMattetitudeMatteStainLipstick</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectMattecentricLipCrayon</t>
-  </si>
-  <si>
-    <t>WardahInstaperfectMatteFitPowderFoundation</t>
-  </si>
-  <si>
-    <t>WardahRefillInstaperfectMatteFitPowderFoundation</t>
-  </si>
-  <si>
-    <t>WardahColorfitVelvetMatteLipMousse</t>
-  </si>
-  <si>
-    <t>EminaMagicPotion</t>
-  </si>
-  <si>
-    <t>EminaGlossyStain</t>
-  </si>
-  <si>
-    <t>EminaCheekLitPressedBlush</t>
-  </si>
-  <si>
-    <t>EminaCheekLitCreamBlush</t>
-  </si>
-  <si>
-    <t>EminaBeautyBlissBbCream</t>
-  </si>
-  <si>
-    <t>EminaBareWithMeMineralCushion</t>
-  </si>
-  <si>
-    <t>EminaBrightStuffLoosePowder</t>
-  </si>
-  <si>
-    <t>EminaPoreRanger</t>
-  </si>
-  <si>
-    <t>EminaDailyMatteLoosePowder</t>
-  </si>
-  <si>
-    <t>EminaPopRougePressedEyeShadow</t>
-  </si>
-  <si>
-    <t>EminaCityChicCcCake</t>
-  </si>
-  <si>
-    <t>EminaStarLashAquaMascara</t>
-  </si>
-  <si>
-    <t>EminaAgentOfBrow</t>
-  </si>
-  <si>
-    <t>EminaEyeDoCrayonPourLesYeux</t>
-  </si>
-  <si>
-    <t>EminaTopSecretEyebrow</t>
-  </si>
-  <si>
-    <t>EminaDoubleAgentEyebrow</t>
-  </si>
-  <si>
-    <t>EminaCreamatteMetallicEdition</t>
-  </si>
-  <si>
-    <t>EminaSoulmatteLipstick</t>
-  </si>
-  <si>
-    <t>EminaSugarRushLipstick</t>
-  </si>
-  <si>
-    <t>EminaCreamytint</t>
-  </si>
-  <si>
-    <t>EminaCreamatte</t>
-  </si>
-  <si>
-    <t>EminaLipCushion</t>
-  </si>
-  <si>
-    <t>EminaTintedLipbalm</t>
-  </si>
-  <si>
-    <t>EminaLiquidLipShine</t>
-  </si>
-  <si>
-    <t>EminaSmoochiesLipbalm</t>
-  </si>
-  <si>
-    <t>SariayuLipstick</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2019HydraLipTint</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2019LiteLipCream</t>
-  </si>
-  <si>
-    <t>SariayuLipCare</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2016DuoLipColor</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2017DuoLipColor</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2018LipCream</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2018LipMetallic</t>
-  </si>
-  <si>
-    <t>SariayuLipColourMatte</t>
-  </si>
-  <si>
-    <t>SariayuCt19LiteLipCream</t>
-  </si>
-  <si>
-    <t>SariayuTrend2017DuoLipColor</t>
-  </si>
-  <si>
-    <t>SariayuLipColorMatte</t>
-  </si>
-  <si>
-    <t>SariayuTwoWayCake</t>
-  </si>
-  <si>
-    <t>SariayuMoisturizer</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2020LipCheek</t>
-  </si>
-  <si>
-    <t>SariayuTwoWayCakeEnergizingAromaticRefill</t>
-  </si>
-  <si>
-    <t>SariayuAlasBedakEnergizingAromatic</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2020CheekPalette</t>
-  </si>
-  <si>
-    <t>SariayuLoosePowder</t>
-  </si>
-  <si>
-    <t>SariayuCreamyFoundation</t>
-  </si>
-  <si>
-    <t>SariayuCompactPowderSpf15</t>
-  </si>
-  <si>
-    <t>SariayuCompactPowder</t>
-  </si>
-  <si>
-    <t>SariayuAlasBedak</t>
-  </si>
-  <si>
-    <t>SariayuBedakJerawatEnergizingAromatic</t>
-  </si>
-  <si>
-    <t>SariayuRefillTwoWayCake</t>
-  </si>
-  <si>
-    <t>SariayuBlushOn</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2015EyelinerPencil</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2020EyeMakeupKit</t>
-  </si>
-  <si>
-    <t>SariayuPensilAlisPro</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2019EyeShadow</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2015Mascara</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend16EyeShadowKit</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend18EyeShadowKit</t>
-  </si>
-  <si>
-    <t>SariayuPensilAlis</t>
-  </si>
-  <si>
-    <t>SariayuTrendWarna2011MoistpomeEyeShadow</t>
-  </si>
-  <si>
-    <t>SariayuColorTrendWarna2011MoistpomeEyeShadowPalette</t>
-  </si>
-  <si>
-    <t>SariayuDuoEyeMakeUp</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2017LiquidEyeShadow</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2016EyeShadow</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend2017EyeShadowKit</t>
-  </si>
-  <si>
-    <t>SariayuColorTrend16Eyeshadow</t>
+    <t>Wardah Everyday Cheek Liptint</t>
+  </si>
+  <si>
+    <t>Wardah Exclusive Matte Lip Cream</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Eye Lip Make Up Remover</t>
+  </si>
+  <si>
+    <t>Wardah Intense Matte Lipstick</t>
+  </si>
+  <si>
+    <t>Wardah Lipstick Longlasting</t>
+  </si>
+  <si>
+    <t>Wardah Longlasting Lipstick</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Optimum Hi Black Liner</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Aqua Lash Mascara</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Eye Shadow Classic</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert The Volume Expert Mascara</t>
+  </si>
+  <si>
+    <t>Wardah Renew You Anti Aging Eye Cream</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Perfectcurl Mascara</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Staylast Liquid Eyeliner</t>
+  </si>
+  <si>
+    <t>Wardah Eye Shadow</t>
+  </si>
+  <si>
+    <t>Wardah Eyexpert Eye Shadow</t>
+  </si>
+  <si>
+    <t>Wardah Acnederm Face Powder</t>
+  </si>
+  <si>
+    <t>Wardah Blush On</t>
+  </si>
+  <si>
+    <t>Wardah Exclusive Liquid Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Exclusive Two Way Cake</t>
+  </si>
+  <si>
+    <t>Wardah Everyday Luminous Compact Powder</t>
+  </si>
+  <si>
+    <t>Wardah Everyday Luminous Face Powder</t>
+  </si>
+  <si>
+    <t>Wardah Refill Lightening Powder Foundation Light Feel</t>
+  </si>
+  <si>
+    <t>Wardah Lightening Powder Foundation Light Feel</t>
+  </si>
+  <si>
+    <t>Wardah Refill Exclusive Two Way Cake</t>
+  </si>
+  <si>
+    <t>Wardah Lightening Powder Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Refill Lightening Powder Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Everyday Luminous Liquid Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Refill Everyday Luminous Two Way Cake</t>
+  </si>
+  <si>
+    <t>Wardah Everyday Shine Free Bb Loose Powder</t>
+  </si>
+  <si>
+    <t>Wardah Lightening Matte Powder</t>
+  </si>
+  <si>
+    <t>Wardah Lightening Bb Cake Powder</t>
+  </si>
+  <si>
+    <t>Wardah Everyday Luminous Two Way Cake</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Porefection Skin Primer</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Mineralight Matte Bb Cushion</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Spotlight Chromatic Eye Palette</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Geniustwist Matic Contour Brow Brushed</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Hypergetic Precise Black Liner</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Mattesetter Lip Matte Paint</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Quick Fix Cover Correct Concealer</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Dynamatic Microsmooth Liner</t>
+  </si>
+  <si>
+    <t>Wardah Refill Instaperfect Mineralight Matte Bb Cushion</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Gloss Chic Lip Crayon</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Mattetitude Matte Stain Lipstick</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Mattecentric Lip Crayon</t>
+  </si>
+  <si>
+    <t>Wardah Instaperfect Matte Fit Powder Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Refill Instaperfect Matte Fit Powder Foundation</t>
+  </si>
+  <si>
+    <t>Wardah Colorfit Velvet Matte Lip Mousse</t>
+  </si>
+  <si>
+    <t>Emina Magic Potion</t>
+  </si>
+  <si>
+    <t>Emina Glossy Stain</t>
+  </si>
+  <si>
+    <t>Emina Cheek Lit Pressed Blush</t>
+  </si>
+  <si>
+    <t>Emina Cheek Lit Cream Blush</t>
+  </si>
+  <si>
+    <t>Emina Beauty Bliss Bb Cream</t>
+  </si>
+  <si>
+    <t>Emina Bare With Me Mineral Cushion</t>
+  </si>
+  <si>
+    <t>Emina Bright Stuff Loose Powder</t>
+  </si>
+  <si>
+    <t>Emina Pore Ranger</t>
+  </si>
+  <si>
+    <t>Emina Daily Matte Loose Powder</t>
+  </si>
+  <si>
+    <t>Emina Pop Rouge Pressed Eye Shadow</t>
+  </si>
+  <si>
+    <t>Emina City Chic Cc Cake</t>
+  </si>
+  <si>
+    <t>Emina Star Lash Aqua Mascara</t>
+  </si>
+  <si>
+    <t>Emina Agent Of Brow</t>
+  </si>
+  <si>
+    <t>Emina Eye Do Crayon Pour Les Yeux</t>
+  </si>
+  <si>
+    <t>Emina Top Secret Eyebrow</t>
+  </si>
+  <si>
+    <t>Emina Double Agent Eyebrow</t>
+  </si>
+  <si>
+    <t>Emina Creamatte Metallic Edition</t>
+  </si>
+  <si>
+    <t>Emina Soulmatte Lipstick</t>
+  </si>
+  <si>
+    <t>Emina Sugar Rush Lipstick</t>
+  </si>
+  <si>
+    <t>Emina Creamytint</t>
+  </si>
+  <si>
+    <t>Emina Creamatte</t>
+  </si>
+  <si>
+    <t>Emina Lip Cushion</t>
+  </si>
+  <si>
+    <t>Emina Tinted Lipbalm</t>
+  </si>
+  <si>
+    <t>Emina Liquid Lip Shine</t>
+  </si>
+  <si>
+    <t>Emina Smoochies Lipbalm</t>
+  </si>
+  <si>
+    <t>Sariayu Lipstick</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2019 Hydra Lip Tint</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2019 Lite Lip Cream</t>
+  </si>
+  <si>
+    <t>Sariayu Lip Care</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2016 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2017 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2018 Lip Cream</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2018 Lip Metallic</t>
+  </si>
+  <si>
+    <t>Sariayu Lip Colour Matte</t>
+  </si>
+  <si>
+    <t>Sariayu Ct 19 Lite Lip Cream</t>
+  </si>
+  <si>
+    <t>Sariayu Trend 2017 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>Sariayu Lip Color Matte</t>
+  </si>
+  <si>
+    <t>Sariayu Two Way Cake</t>
+  </si>
+  <si>
+    <t>Sariayu Moisturizer</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2020 Lip Cheek</t>
+  </si>
+  <si>
+    <t>Sariayu Two Way Cake Energizing Aromatic Refill</t>
+  </si>
+  <si>
+    <t>Sariayu Alas Bedak Energizing Aromatic</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2020 Cheek Palette</t>
+  </si>
+  <si>
+    <t>Sariayu Loose Powder</t>
+  </si>
+  <si>
+    <t>Sariayu Creamy Foundation</t>
+  </si>
+  <si>
+    <t>Sariayu Compact Powder Spf 15</t>
+  </si>
+  <si>
+    <t>Sariayu Compact Powder</t>
+  </si>
+  <si>
+    <t>Sariayu Alas Bedak</t>
+  </si>
+  <si>
+    <t>Sariayu Bedak Jerawat Energizing Aromatic</t>
+  </si>
+  <si>
+    <t>Sariayu Refill Two Way Cake</t>
+  </si>
+  <si>
+    <t>Sariayu Blush On</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2015 Eyeliner Pencil</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2020 Eye Makeup Kit</t>
+  </si>
+  <si>
+    <t>Sariayu Pensil Alis Pro</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2019 Eye Shadow</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2015 Mascara</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 16 Eye Shadow Kit</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 18 Eye Shadow Kit</t>
+  </si>
+  <si>
+    <t>Sariayu Pensil Alis</t>
+  </si>
+  <si>
+    <t>Sariayu Trend Warna 2011 Moistpome Eye Shadow</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend Warna 2011 Moistpome Eye Shadow Palette</t>
+  </si>
+  <si>
+    <t>Sariayu Duo Eye Make Up</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2017 Liquid Eye Shadow</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2016 Eye Shadow</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 2017 Eye Shadow Kit</t>
+  </si>
+  <si>
+    <t>Sariayu Color Trend 16 Eyeshadow</t>
   </si>
   <si>
     <t>null</t>

</xml_diff>